<commit_message>
Se modifico el metodo cargarArchivoAsistencia, ahora no es necesario poner el nombre en duro ;)
</commit_message>
<xml_diff>
--- a/ProyectoPermanencia.Presentacion/Uploads/Asistencia.xlsx
+++ b/ProyectoPermanencia.Presentacion/Uploads/Asistencia.xlsx
@@ -1,32 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturoguerra/Dropbox/CITT/Permanencia/Sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raide\Desktop\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24220" windowHeight="10820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="dkjshfdsjhfdjks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dkjshfdsjhfdjks!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -565,23 +562,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD43523"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>7198787</v>
       </c>
@@ -627,7 +624,7 @@
         <v>0.95238095238095233</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>8438011</v>
       </c>
@@ -650,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>8438011</v>
       </c>
@@ -673,7 +670,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>8438011</v>
       </c>
@@ -696,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>8454451</v>
       </c>
@@ -719,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>8454451</v>
       </c>
@@ -742,7 +739,7 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8454451</v>
       </c>
@@ -765,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8667437</v>
       </c>
@@ -788,7 +785,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8667437</v>
       </c>
@@ -811,7 +808,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8667437</v>
       </c>
@@ -834,7 +831,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8667437</v>
       </c>
@@ -857,7 +854,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8667437</v>
       </c>
@@ -880,7 +877,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8667437</v>
       </c>
@@ -903,7 +900,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>8667437</v>
       </c>
@@ -926,7 +923,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>8667437</v>
       </c>
@@ -949,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8667437</v>
       </c>
@@ -972,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8669508</v>
       </c>
@@ -995,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>8669508</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>8669508</v>
       </c>
@@ -1041,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>8669508</v>
       </c>
@@ -1064,7 +1061,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>8669508</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>8669508</v>
       </c>
@@ -1110,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>8669508</v>
       </c>
@@ -1133,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8669508</v>
       </c>

</xml_diff>